<commit_message>
fix bugs the thanh vien, the ưu đãi
</commit_message>
<xml_diff>
--- a/TMTDentalAPI/ClientApp/src/assets/files/File_mau_the_thanh_vien.xlsx
+++ b/TMTDentalAPI/ClientApp/src/assets/files/File_mau_the_thanh_vien.xlsx
@@ -24,36 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Số ID thẻ</t>
   </si>
   <si>
     <t>Hạng thẻ</t>
-  </si>
-  <si>
-    <t>TTV1234567</t>
-  </si>
-  <si>
-    <t>Vàng</t>
-  </si>
-  <si>
-    <t>TTV1234568</t>
-  </si>
-  <si>
-    <t>Bạc</t>
-  </si>
-  <si>
-    <t>TTV1234569</t>
-  </si>
-  <si>
-    <t>Đồng</t>
-  </si>
-  <si>
-    <t>TTV123</t>
-  </si>
-  <si>
-    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -380,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,38 +375,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
done us and fix some bug
</commit_message>
<xml_diff>
--- a/TMTDentalAPI/ClientApp/src/assets/files/File_mau_the_thanh_vien.xlsx
+++ b/TMTDentalAPI/ClientApp/src/assets/files/File_mau_the_thanh_vien.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\TMTDentalAPI\ClientApp\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I710700\Desktop\Source\TDental\TMTDentalAPI\ClientApp\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -358,8 +358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>